<commit_message>
Modifications to execute the program.
</commit_message>
<xml_diff>
--- a/source/excel_files/Network parameters.xlsx
+++ b/source/excel_files/Network parameters.xlsx
@@ -1906,12 +1906,12 @@
     <row r="5" ht="43.5" customHeight="1" s="50">
       <c r="A5" s="35" t="inlineStr">
         <is>
-          <t>FRECUENCY POINTS TO BE ANALYZED</t>
+          <t>ANALYSIS FREQUENCY STEP</t>
         </is>
       </c>
       <c r="B5" s="36" t="inlineStr">
         <is>
-          <t>500 Hz,5 KHz</t>
+          <t>50.00 Hz,60.00 Hz,70.00 Hz,80.00 Hz,90.00 Hz,100.00 Hz,110.00 Hz,120.00 Hz,130.00 Hz,140.00 Hz,150.00 Hz,160.00 Hz,170.00 Hz,180.00 Hz,190.00 Hz,200.00 Hz,210.00 Hz,220.00 Hz,230.00 Hz,240.00 Hz,250.00 Hz,260.00 Hz,270.00 Hz,280.00 Hz,290.00 Hz,300.00 Hz,310.00 Hz,320.00 Hz,330.00 Hz,340.00 Hz,350.00 Hz,360.00 Hz,370.00 Hz,380.00 Hz,390.00 Hz,400.00 Hz,410.00 Hz,420.00 Hz,430.00 Hz,440.00 Hz,450.00 Hz,460.00 Hz,470.00 Hz,480.00 Hz,490.00 Hz,500.00 Hz,510.00 Hz,520.00 Hz,530.00 Hz,540.00 Hz,550.00 Hz,560.00 Hz,570.00 Hz,580.00 Hz,590.00 Hz,600.00 Hz,610.00 Hz,620.00 Hz,630.00 Hz,640.00 Hz,650.00 Hz,660.00 Hz,670.00 Hz,680.00 Hz,690.00 Hz,700.00 Hz,710.00 Hz,720.00 Hz,730.00 Hz,740.00 Hz,750.00 Hz,760.00 Hz,770.00 Hz,780.00 Hz,790.00 Hz,800.00 Hz,810.00 Hz,820.00 Hz,830.00 Hz,840.00 Hz,850.00 Hz,860.00 Hz,870.00 Hz,880.00 Hz,890.00 Hz,900.00 Hz,910.00 Hz,920.00 Hz,930.00 Hz,940.00 Hz,950.00 Hz,960.00 Hz,970.00 Hz,980.00 Hz,990.00 Hz,1.00 KHz,1.01 KHz,1.02 KHz,1.03 KHz,1.04 KHz,1.05 KHz,1.06 KHz,1.07 KHz,1.08 KHz,1.09 KHz,1.10 KHz,1.11 KHz,1.12 KHz,1.13 KHz,1.14 KHz,1.15 KHz,1.16 KHz,1.17 KHz,1.18 KHz,1.19 KHz,1.20 KHz,1.21 KHz,1.22 KHz,1.23 KHz,1.24 KHz,1.25 KHz,1.26 KHz,1.27 KHz,1.28 KHz,1.29 KHz,1.30 KHz,1.31 KHz,1.32 KHz,1.33 KHz,1.34 KHz,1.35 KHz,1.36 KHz,1.37 KHz,1.38 KHz,1.39 KHz,1.40 KHz,1.41 KHz,1.42 KHz,1.43 KHz,1.44 KHz,1.45 KHz,1.46 KHz,1.47 KHz,1.48 KHz,1.49 KHz,1.50 KHz,1.51 KHz,1.52 KHz,1.53 KHz,1.54 KHz,1.55 KHz,1.56 KHz,1.57 KHz,1.58 KHz,1.59 KHz,1.60 KHz,1.61 KHz,1.62 KHz,1.63 KHz,1.64 KHz,1.65 KHz,1.66 KHz,1.67 KHz,1.68 KHz,1.69 KHz,1.70 KHz,1.71 KHz,1.72 KHz,1.73 KHz,1.74 KHz,1.75 KHz,1.76 KHz,1.77 KHz,1.78 KHz,1.79 KHz,1.80 KHz,1.81 KHz,1.82 KHz,1.83 KHz,1.84 KHz,1.85 KHz,1.86 KHz,1.87 KHz,1.88 KHz,1.89 KHz,1.90 KHz,1.91 KHz,1.92 KHz,1.93 KHz,1.94 KHz,1.95 KHz,1.96 KHz,1.97 KHz,1.98 KHz,1.99 KHz,2.00 KHz,2.01 KHz,2.02 KHz,2.03 KHz,2.04 KHz,2.05 KHz,2.06 KHz,2.07 KHz,2.08 KHz,2.09 KHz,2.10 KHz,2.11 KHz,2.12 KHz,2.13 KHz,2.14 KHz,2.15 KHz,2.16 KHz,2.17 KHz,2.18 KHz,2.19 KHz,2.20 KHz,2.21 KHz,2.22 KHz,2.23 KHz,2.24 KHz,2.25 KHz,2.26 KHz,2.27 KHz,2.28 KHz,2.29 KHz,2.30 KHz,2.31 KHz,2.32 KHz,2.33 KHz,2.34 KHz,2.35 KHz,2.36 KHz,2.37 KHz,2.38 KHz,2.39 KHz,2.40 KHz,2.41 KHz,2.42 KHz,2.43 KHz,2.44 KHz,2.45 KHz,2.46 KHz,2.47 KHz,2.48 KHz,2.49 KHz,2.50 KHz,2.51 KHz,2.52 KHz,2.53 KHz,2.54 KHz,2.55 KHz,2.56 KHz,2.57 KHz,2.58 KHz,2.59 KHz,2.60 KHz,2.61 KHz,2.62 KHz,2.63 KHz,2.64 KHz,2.65 KHz,2.66 KHz,2.67 KHz,2.68 KHz,2.69 KHz,2.70 KHz,2.71 KHz,2.72 KHz,2.73 KHz,2.74 KHz,2.75 KHz,2.76 KHz,2.77 KHz,2.78 KHz,2.79 KHz,2.80 KHz,2.81 KHz,2.82 KHz,2.83 KHz,2.84 KHz,2.85 KHz,2.86 KHz,2.87 KHz,2.88 KHz,2.89 KHz,2.90 KHz,2.91 KHz,2.92 KHz,2.93 KHz,2.94 KHz,2.95 KHz,2.96 KHz,2.97 KHz,2.98 KHz,2.99 KHz,3.00 KHz,3.01 KHz,3.02 KHz,3.03 KHz,3.04 KHz,3.05 KHz,3.06 KHz,3.07 KHz,3.08 KHz,3.09 KHz,3.10 KHz,3.11 KHz,3.12 KHz,3.13 KHz,3.14 KHz,3.15 KHz,3.16 KHz,3.17 KHz,3.18 KHz,3.19 KHz,3.20 KHz,3.21 KHz,3.22 KHz,3.23 KHz,3.24 KHz,3.25 KHz,3.26 KHz,3.27 KHz,3.28 KHz,3.29 KHz,3.30 KHz,3.31 KHz,3.32 KHz,3.33 KHz,3.34 KHz,3.35 KHz,3.36 KHz,3.37 KHz,3.38 KHz,3.39 KHz,3.40 KHz,3.41 KHz,3.42 KHz,3.43 KHz,3.44 KHz,3.45 KHz,3.46 KHz,3.47 KHz,3.48 KHz,3.49 KHz,3.50 KHz,3.51 KHz,3.52 KHz,3.53 KHz,3.54 KHz,3.55 KHz,3.56 KHz,3.57 KHz,3.58 KHz,3.59 KHz,3.60 KHz,3.61 KHz,3.62 KHz,3.63 KHz,3.64 KHz,3.65 KHz,3.66 KHz,3.67 KHz,3.68 KHz,3.69 KHz,3.70 KHz,3.71 KHz,3.72 KHz,3.73 KHz,3.74 KHz,3.75 KHz,3.76 KHz,3.77 KHz,3.78 KHz,3.79 KHz,3.80 KHz,3.81 KHz,3.82 KHz,3.83 KHz,3.84 KHz,3.85 KHz,3.86 KHz,3.87 KHz,3.88 KHz,3.89 KHz,3.90 KHz,3.91 KHz,3.92 KHz,3.93 KHz,3.94 KHz,3.95 KHz,3.96 KHz,3.97 KHz,3.98 KHz,3.99 KHz,4.00 KHz,4.01 KHz,4.02 KHz,4.03 KHz,4.04 KHz,4.05 KHz,4.06 KHz,4.07 KHz,4.08 KHz,4.09 KHz,4.10 KHz,4.11 KHz,4.12 KHz,4.13 KHz,4.14 KHz,4.15 KHz,4.16 KHz,4.17 KHz,4.18 KHz,4.19 KHz,4.20 KHz,4.21 KHz,4.22 KHz,4.23 KHz,4.24 KHz,4.25 KHz,4.26 KHz,4.27 KHz,4.28 KHz,4.29 KHz,4.30 KHz,4.31 KHz,4.32 KHz,4.33 KHz,4.34 KHz,4.35 KHz,4.36 KHz,4.37 KHz,4.38 KHz,4.39 KHz,4.40 KHz,4.41 KHz,4.42 KHz,4.43 KHz,4.44 KHz,4.45 KHz,4.46 KHz,4.47 KHz,4.48 KHz,4.49 KHz,4.50 KHz,4.51 KHz,4.52 KHz,4.53 KHz,4.54 KHz,4.55 KHz,4.56 KHz,4.57 KHz,4.58 KHz,4.59 KHz,4.60 KHz,4.61 KHz,4.62 KHz,4.63 KHz,4.64 KHz,4.65 KHz,4.66 KHz,4.67 KHz,4.68 KHz,4.69 KHz,4.70 KHz,4.71 KHz,4.72 KHz,4.73 KHz,4.74 KHz,4.75 KHz,4.76 KHz,4.77 KHz,4.78 KHz,4.79 KHz,4.80 KHz,4.81 KHz,4.82 KHz,4.83 KHz,4.84 KHz,4.85 KHz,4.86 KHz,4.87 KHz,4.88 KHz,4.89 KHz,4.90 KHz,4.91 KHz,4.92 KHz,4.93 KHz,4.94 KHz,4.95 KHz,4.96 KHz,4.97 KHz,4.98 KHz,4.99 KHz,5.00 KHz,5.01 KHz,5.02 KHz,5.03 KHz,5.04 KHz,5.05 KHz,5.06 KHz,5.07 KHz,5.08 KHz,5.09 KHz,5.10 KHz,5.11 KHz,5.12 KHz,5.13 KHz,5.14 KHz,5.15 KHz,5.16 KHz,5.17 KHz,5.18 KHz,5.19 KHz,5.20 KHz,5.21 KHz,5.22 KHz,5.23 KHz,5.24 KHz,5.25 KHz,5.26 KHz,5.27 KHz,5.28 KHz,5.29 KHz,5.30 KHz,5.31 KHz,5.32 KHz,5.33 KHz,5.34 KHz,5.35 KHz,5.36 KHz,5.37 KHz,5.38 KHz,5.39 KHz,5.40 KHz,5.41 KHz,5.42 KHz,5.43 KHz,5.44 KHz,5.45 KHz,5.46 KHz,5.47 KHz,5.48 KHz,5.49 KHz,5.50 KHz,5.51 KHz,5.52 KHz,5.53 KHz,5.54 KHz,5.55 KHz,5.56 KHz,5.57 KHz,5.58 KHz,5.59 KHz,5.60 KHz,5.61 KHz,5.62 KHz,5.63 KHz,5.64 KHz,5.65 KHz,5.66 KHz,5.67 KHz,5.68 KHz,5.69 KHz,5.70 KHz,5.71 KHz,5.72 KHz,5.73 KHz,5.74 KHz,5.75 KHz,5.76 KHz,5.77 KHz,5.78 KHz,5.79 KHz,5.80 KHz,5.81 KHz,5.82 KHz,5.83 KHz,5.84 KHz,5.85 KHz,5.86 KHz,5.87 KHz,5.88 KHz,5.89 KHz,5.90 KHz,5.91 KHz,5.92 KHz,5.93 KHz,5.94 KHz,5.95 KHz,5.96 KHz,5.97 KHz,5.98 KHz,5.99 KHz,6.00 KHz,6.01 KHz,6.02 KHz,6.03 KHz,6.04 KHz,6.05 KHz,6.06 KHz,6.07 KHz,6.08 KHz,6.09 KHz,6.10 KHz,6.11 KHz,6.12 KHz,6.13 KHz,6.14 KHz,6.15 KHz,6.16 KHz,6.17 KHz,6.18 KHz,6.19 KHz,6.20 KHz,6.21 KHz,6.22 KHz,6.23 KHz,6.24 KHz,6.25 KHz,6.26 KHz,6.27 KHz,6.28 KHz,6.29 KHz,6.30 KHz,6.31 KHz,6.32 KHz,6.33 KHz,6.34 KHz,6.35 KHz,6.36 KHz,6.37 KHz,6.38 KHz,6.39 KHz,6.40 KHz,6.41 KHz,6.42 KHz,6.43 KHz,6.44 KHz,6.45 KHz,6.46 KHz,6.47 KHz,6.48 KHz,6.49 KHz,6.50 KHz,6.51 KHz,6.52 KHz,6.53 KHz,6.54 KHz,6.55 KHz,6.56 KHz,6.57 KHz,6.58 KHz,6.59 KHz,6.60 KHz,6.61 KHz,6.62 KHz,6.63 KHz,6.64 KHz,6.65 KHz,6.66 KHz,6.67 KHz,6.68 KHz,6.69 KHz,6.70 KHz,6.71 KHz,6.72 KHz,6.73 KHz,6.74 KHz,6.75 KHz,6.76 KHz,6.77 KHz,6.78 KHz,6.79 KHz,6.80 KHz,6.81 KHz,6.82 KHz,6.83 KHz,6.84 KHz,6.85 KHz,6.86 KHz,6.87 KHz,6.88 KHz,6.89 KHz,6.90 KHz,6.91 KHz,6.92 KHz,6.93 KHz,6.94 KHz,6.95 KHz,6.96 KHz,6.97 KHz,6.98 KHz,6.99 KHz,7.00 KHz,7.01 KHz,7.02 KHz,7.03 KHz,7.04 KHz,7.05 KHz,7.06 KHz,7.07 KHz,7.08 KHz,7.09 KHz,7.10 KHz,7.11 KHz,7.12 KHz,7.13 KHz,7.14 KHz,7.15 KHz,7.16 KHz,7.17 KHz,7.18 KHz,7.19 KHz,7.20 KHz,7.21 KHz,7.22 KHz,7.23 KHz,7.24 KHz,7.25 KHz,7.26 KHz,7.27 KHz,7.28 KHz,7.29 KHz,7.30 KHz,7.31 KHz,7.32 KHz,7.33 KHz,7.34 KHz,7.35 KHz,7.36 KHz,7.37 KHz,7.38 KHz,7.39 KHz,7.40 KHz,7.41 KHz,7.42 KHz,7.43 KHz,7.44 KHz,7.45 KHz,7.46 KHz,7.47 KHz,7.48 KHz,7.49 KHz,7.50 KHz,7.51 KHz,7.52 KHz,7.53 KHz,7.54 KHz,7.55 KHz,7.56 KHz,7.57 KHz,7.58 KHz,7.59 KHz,7.60 KHz,7.61 KHz,7.62 KHz,7.63 KHz,7.64 KHz,7.65 KHz,7.66 KHz,7.67 KHz,7.68 KHz,7.69 KHz,7.70 KHz,7.71 KHz,7.72 KHz,7.73 KHz,7.74 KHz,7.75 KHz,7.76 KHz,7.77 KHz,7.78 KHz,7.79 KHz,7.80 KHz,7.81 KHz,7.82 KHz,7.83 KHz,7.84 KHz,7.85 KHz,7.86 KHz,7.87 KHz,7.88 KHz,7.89 KHz,7.90 KHz,7.91 KHz,7.92 KHz,7.93 KHz,7.94 KHz,7.95 KHz,7.96 KHz,7.97 KHz,7.98 KHz,7.99 KHz,8.00 KHz,8.01 KHz,8.02 KHz,8.03 KHz,8.04 KHz,8.05 KHz,8.06 KHz,8.07 KHz,8.08 KHz,8.09 KHz,8.10 KHz,8.11 KHz,8.12 KHz,8.13 KHz,8.14 KHz,8.15 KHz,8.16 KHz,8.17 KHz,8.18 KHz,8.19 KHz,8.20 KHz,8.21 KHz,8.22 KHz,8.23 KHz,8.24 KHz,8.25 KHz,8.26 KHz,8.27 KHz,8.28 KHz,8.29 KHz,8.30 KHz,8.31 KHz,8.32 KHz,8.33 KHz,8.34 KHz,8.35 KHz,8.36 KHz,8.37 KHz,8.38 KHz,8.39 KHz,8.40 KHz,8.41 KHz,8.42 KHz,8.43 KHz,8.44 KHz,8.45 KHz,8.46 KHz,8.47 KHz,8.48 KHz,8.49 KHz,8.50 KHz,8.51 KHz,8.52 KHz,8.53 KHz,8.54 KHz,8.55 KHz,8.56 KHz,8.57 KHz,8.58 KHz,8.59 KHz,8.60 KHz,8.61 KHz,8.62 KHz,8.63 KHz,8.64 KHz,8.65 KHz,8.66 KHz,8.67 KHz,8.68 KHz,8.69 KHz,8.70 KHz,8.71 KHz,8.72 KHz,8.73 KHz,8.74 KHz,8.75 KHz,8.76 KHz,8.77 KHz,8.78 KHz,8.79 KHz,8.80 KHz,8.81 KHz,8.82 KHz,8.83 KHz,8.84 KHz,8.85 KHz,8.86 KHz,8.87 KHz,8.88 KHz,8.89 KHz,8.90 KHz,8.91 KHz,8.92 KHz,8.93 KHz,8.94 KHz,8.95 KHz,8.96 KHz,8.97 KHz,8.98 KHz,8.99 KHz,9.00 KHz,9.01 KHz,9.02 KHz,9.03 KHz,9.04 KHz,9.05 KHz,9.06 KHz,9.07 KHz,9.08 KHz,9.09 KHz,9.10 KHz,9.11 KHz,9.12 KHz,9.13 KHz,9.14 KHz,9.15 KHz,9.16 KHz,9.17 KHz,9.18 KHz,9.19 KHz,9.20 KHz,9.21 KHz,9.22 KHz,9.23 KHz,9.24 KHz,9.25 KHz,9.26 KHz,9.27 KHz,9.28 KHz,9.29 KHz,9.30 KHz,9.31 KHz,9.32 KHz,9.33 KHz,9.34 KHz,9.35 KHz,9.36 KHz,9.37 KHz,9.38 KHz,9.39 KHz,9.40 KHz,9.41 KHz,9.42 KHz,9.43 KHz,9.44 KHz,9.45 KHz,9.46 KHz,9.47 KHz,9.48 KHz,9.49 KHz,9.50 KHz,9.51 KHz,9.52 KHz,9.53 KHz,9.54 KHz,9.55 KHz,9.56 KHz,9.57 KHz,9.58 KHz,9.59 KHz,9.60 KHz,9.61 KHz,9.62 KHz,9.63 KHz,9.64 KHz,9.65 KHz,9.66 KHz,9.67 KHz,9.68 KHz,9.69 KHz,9.70 KHz,9.71 KHz,9.72 KHz,9.73 KHz,9.74 KHz,9.75 KHz,9.76 KHz,9.77 KHz,9.78 KHz,9.79 KHz,9.80 KHz,9.81 KHz,9.82 KHz,9.83 KHz,9.84 KHz,9.85 KHz,9.86 KHz,9.87 KHz,9.88 KHz,9.89 KHz,9.90 KHz,9.91 KHz,9.92 KHz,9.93 KHz,9.94 KHz,9.95 KHz,9.96 KHz,9.97 KHz,9.98 KHz,9.99 KHz,10.00 KHz,10.01 KHz,10.02 KHz,10.03 KHz,10.04 KHz,10.05 KHz,10.06 KHz,10.07 KHz,10.08 KHz,10.09 KHz,10.10 KHz,10.11 KHz,10.12 KHz,10.13 KHz,10.14 KHz,10.15 KHz,10.16 KHz,10.17 KHz,10.18 KHz,10.19 KHz,10.20 KHz,10.21 KHz,10.22 KHz,10.23 KHz,10.24 KHz,10.25 KHz,10.26 KHz,10.27 KHz,10.28 KHz,10.29 KHz,10.30 KHz,10.31 KHz,10.32 KHz,10.33 KHz,10.34 KHz,10.35 KHz,10.36 KHz,10.37 KHz,10.38 KHz,10.39 KHz,10.40 KHz,10.41 KHz,10.42 KHz,10.43 KHz,10.44 KHz,10.45 KHz,10.46 KHz,10.47 KHz,10.48 KHz,10.49 KHz,10.50 KHz,10.51 KHz,10.52 KHz,10.53 KHz,10.54 KHz,10.55 KHz,10.56 KHz,10.57 KHz,10.58 KHz,10.59 KHz,10.60 KHz,10.61 KHz,10.62 KHz,10.63 KHz,10.64 KHz,10.65 KHz,10.66 KHz,10.67 KHz,10.68 KHz,10.69 KHz,10.70 KHz,10.71 KHz,10.72 KHz,10.73 KHz,10.74 KHz,10.75 KHz,10.76 KHz,10.77 KHz,10.78 KHz,10.79 KHz,10.80 KHz,10.81 KHz,10.82 KHz,10.83 KHz,10.84 KHz,10.85 KHz,10.86 KHz,10.87 KHz,10.88 KHz,10.89 KHz,10.90 KHz,10.91 KHz,10.92 KHz,10.93 KHz,10.94 KHz,10.95 KHz,10.96 KHz,10.97 KHz,10.98 KHz,10.99 KHz,11.00 KHz,11.01 KHz,11.02 KHz,11.03 KHz,11.04 KHz,11.05 KHz,11.06 KHz,11.07 KHz,11.08 KHz,11.09 KHz,11.10 KHz,11.11 KHz,11.12 KHz,11.13 KHz,11.14 KHz,11.15 KHz,11.16 KHz,11.17 KHz,11.18 KHz,11.19 KHz,11.20 KHz,11.21 KHz,11.22 KHz,11.23 KHz,11.24 KHz,11.25 KHz,11.26 KHz,11.27 KHz,11.28 KHz,11.29 KHz,11.30 KHz,11.31 KHz,11.32 KHz,11.33 KHz,11.34 KHz,11.35 KHz,11.36 KHz,11.37 KHz,11.38 KHz,11.39 KHz,11.40 KHz,11.41 KHz,11.42 KHz,11.43 KHz,11.44 KHz,11.45 KHz,11.46 KHz,11.47 KHz,11.48 KHz,11.49 KHz,11.50 KHz,11.51 KHz,11.52 KHz,11.53 KHz,11.54 KHz,11.55 KHz,11.56 KHz,11.57 KHz,11.58 KHz,11.59 KHz,11.60 KHz,11.61 KHz,11.62 KHz,11.63 KHz,11.64 KHz,11.65 KHz,11.66 KHz,11.67 KHz,11.68 KHz,11.69 KHz,11.70 KHz,11.71 KHz,11.72 KHz,11.73 KHz,11.74 KHz,11.75 KHz,11.76 KHz,11.77 KHz,11.78 KHz,11.79 KHz,11.80 KHz,11.81 KHz,11.82 KHz,11.83 KHz,11.84 KHz,11.85 KHz,11.86 KHz,11.87 KHz,11.88 KHz,11.89 KHz,11.90 KHz,11.91 KHz,11.92 KHz,11.93 KHz,11.94 KHz,11.95 KHz,11.96 KHz,11.97 KHz,11.98 KHz,11.99 KHz,12.00 KHz,12.01 KHz,12.02 KHz,12.03 KHz,12.04 KHz,12.05 KHz,12.06 KHz,12.07 KHz,12.08 KHz,12.09 KHz,12.10 KHz,12.11 KHz,12.12 KHz,12.13 KHz,12.14 KHz,12.15 KHz,12.16 KHz,12.17 KHz,12.18 KHz,12.19 KHz,12.20 KHz,12.21 KHz,12.22 KHz,12.23 KHz,12.24 KHz,12.25 KHz,12.26 KHz,12.27 KHz,12.28 KHz,12.29 KHz,12.30 KHz,12.31 KHz,12.32 KHz,12.33 KHz,12.34 KHz,12.35 KHz,12.36 KHz,12.37 KHz,12.38 KHz,12.39 KHz,12.40 KHz,12.41 KHz,12.42 KHz,12.43 KHz,12.44 KHz,12.45 KHz,12.46 KHz,12.47 KHz,12.48 KHz,12.49 KHz,12.50 KHz,12.51 KHz,12.52 KHz,12.53 KHz,12.54 KHz,12.55 KHz,12.56 KHz,12.57 KHz,12.58 KHz,12.59 KHz,12.60 KHz,12.61 KHz,12.62 KHz,12.63 KHz,12.64 KHz,12.65 KHz,12.66 KHz,12.67 KHz,12.68 KHz,12.69 KHz,12.70 KHz,12.71 KHz,12.72 KHz,12.73 KHz,12.74 KHz,12.75 KHz,12.76 KHz,12.77 KHz,12.78 KHz,12.79 KHz,12.80 KHz,12.81 KHz,12.82 KHz,12.83 KHz,12.84 KHz,12.85 KHz,12.86 KHz,12.87 KHz,12.88 KHz,12.89 KHz,12.90 KHz,12.91 KHz,12.92 KHz,12.93 KHz,12.94 KHz,12.95 KHz,12.96 KHz,12.97 KHz,12.98 KHz,12.99 KHz,13.00 KHz,13.01 KHz,13.02 KHz,13.03 KHz,13.04 KHz,13.05 KHz,13.06 KHz,13.07 KHz,13.08 KHz,13.09 KHz,13.10 KHz,13.11 KHz,13.12 KHz,13.13 KHz,13.14 KHz,13.15 KHz,13.16 KHz,13.17 KHz,13.18 KHz,13.19 KHz,13.20 KHz,13.21 KHz,13.22 KHz,13.23 KHz,13.24 KHz,13.25 KHz,13.26 KHz,13.27 KHz,13.28 KHz,13.29 KHz,13.30 KHz,13.31 KHz,13.32 KHz,13.33 KHz,13.34 KHz,13.35 KHz,13.36 KHz,13.37 KHz,13.38 KHz,13.39 KHz,13.40 KHz,13.41 KHz,13.42 KHz,13.43 KHz,13.44 KHz,13.45 KHz,13.46 KHz,13.47 KHz,13.48 KHz,13.49 KHz,13.50 KHz,13.51 KHz,13.52 KHz,13.53 KHz,13.54 KHz,13.55 KHz,13.56 KHz,13.57 KHz,13.58 KHz,13.59 KHz,13.60 KHz,13.61 KHz,13.62 KHz,13.63 KHz,13.64 KHz,13.65 KHz,13.66 KHz,13.67 KHz,13.68 KHz,13.69 KHz,13.70 KHz,13.71 KHz,13.72 KHz,13.73 KHz,13.74 KHz,13.75 KHz,13.76 KHz,13.77 KHz,13.78 KHz,13.79 KHz,13.80 KHz,13.81 KHz,13.82 KHz,13.83 KHz,13.84 KHz,13.85 KHz,13.86 KHz,13.87 KHz,13.88 KHz,13.89 KHz,13.90 KHz,13.91 KHz,13.92 KHz,13.93 KHz,13.94 KHz,13.95 KHz,13.96 KHz,13.97 KHz,13.98 KHz,13.99 KHz,14.00 KHz,14.01 KHz,14.02 KHz,14.03 KHz,14.04 KHz,14.05 KHz,14.06 KHz,14.07 KHz,14.08 KHz,14.09 KHz,14.10 KHz,14.11 KHz,14.12 KHz,14.13 KHz,14.14 KHz,14.15 KHz,14.16 KHz,14.17 KHz,14.18 KHz,14.19 KHz,14.20 KHz,14.21 KHz,14.22 KHz,14.23 KHz,14.24 KHz,14.25 KHz,14.26 KHz,14.27 KHz,14.28 KHz,14.29 KHz,14.30 KHz,14.31 KHz,14.32 KHz,14.33 KHz,14.34 KHz,14.35 KHz,14.36 KHz,14.37 KHz,14.38 KHz,14.39 KHz,14.40 KHz,14.41 KHz,14.42 KHz,14.43 KHz,14.44 KHz,14.45 KHz,14.46 KHz,14.47 KHz,14.48 KHz,14.49 KHz,14.50 KHz,14.51 KHz,14.52 KHz,14.53 KHz,14.54 KHz,14.55 KHz,14.56 KHz,14.57 KHz,14.58 KHz,14.59 KHz,14.60 KHz,14.61 KHz,14.62 KHz,14.63 KHz,14.64 KHz,14.65 KHz,14.66 KHz,14.67 KHz,14.68 KHz,14.69 KHz,14.70 KHz,14.71 KHz,14.72 KHz,14.73 KHz,14.74 KHz,14.75 KHz,14.76 KHz,14.77 KHz,14.78 KHz,14.79 KHz,14.80 KHz,14.81 KHz,14.82 KHz,14.83 KHz,14.84 KHz,14.85 KHz,14.86 KHz,14.87 KHz,14.88 KHz,14.89 KHz,14.90 KHz,14.91 KHz,14.92 KHz,14.93 KHz,14.94 KHz,14.95 KHz,14.96 KHz,14.97 KHz,14.98 KHz,14.99 KHz,15.00 KHz,15.01 KHz,15.02 KHz,15.03 KHz,15.04 KHz,15.05 KHz,15.06 KHz,15.07 KHz,15.08 KHz,15.09 KHz,15.10 KHz,15.11 KHz,15.12 KHz,15.13 KHz,15.14 KHz,15.15 KHz,15.16 KHz,15.17 KHz,15.18 KHz,15.19 KHz,15.20 KHz,15.21 KHz,15.22 KHz,15.23 KHz,15.24 KHz,15.25 KHz,15.26 KHz,15.27 KHz,15.28 KHz,15.29 KHz,15.30 KHz,15.31 KHz,15.32 KHz,15.33 KHz,15.34 KHz,15.35 KHz,15.36 KHz,15.37 KHz,15.38 KHz,15.39 KHz,15.40 KHz,15.41 KHz,15.42 KHz,15.43 KHz,15.44 KHz,15.45 KHz,15.46 KHz,15.47 KHz,15.48 KHz,15.49 KHz,15.50 KHz,15.51 KHz,15.52 KHz,15.53 KHz,15.54 KHz,15.55 KHz,15.56 KHz,15.57 KHz,15.58 KHz,15.59 KHz,15.60 KHz,15.61 KHz,15.62 KHz,15.63 KHz,15.64 KHz,15.65 KHz,15.66 KHz,15.67 KHz,15.68 KHz,15.69 KHz,15.70 KHz,15.71 KHz,15.72 KHz,15.73 KHz,15.74 KHz,15.75 KHz,15.76 KHz,15.77 KHz,15.78 KHz,15.79 KHz,15.80 KHz,15.81 KHz,15.82 KHz,15.83 KHz,15.84 KHz,15.85 KHz,15.86 KHz,15.87 KHz,15.88 KHz,15.89 KHz,15.90 KHz,15.91 KHz,15.92 KHz,15.93 KHz,15.94 KHz,15.95 KHz,15.96 KHz,15.97 KHz,15.98 KHz,15.99 KHz,16.00 KHz,16.01 KHz,16.02 KHz,16.03 KHz,16.04 KHz,16.05 KHz,16.06 KHz,16.07 KHz,16.08 KHz,16.09 KHz,16.10 KHz,16.11 KHz,16.12 KHz,16.13 KHz,16.14 KHz,16.15 KHz,16.16 KHz,16.17 KHz,16.18 KHz,16.19 KHz,16.20 KHz,16.21 KHz,16.22 KHz,16.23 KHz,16.24 KHz,16.25 KHz,16.26 KHz,16.27 KHz,16.28 KHz,16.29 KHz,16.30 KHz,16.31 KHz,16.32 KHz,16.33 KHz,16.34 KHz,16.35 KHz,16.36 KHz,16.37 KHz,16.38 KHz,16.39 KHz,16.40 KHz,16.41 KHz,16.42 KHz,16.43 KHz,16.44 KHz,16.45 KHz,16.46 KHz,16.47 KHz,16.48 KHz,16.49 KHz,16.50 KHz,16.51 KHz,16.52 KHz,16.53 KHz,16.54 KHz,16.55 KHz,16.56 KHz,16.57 KHz,16.58 KHz,16.59 KHz,16.60 KHz,16.61 KHz,16.62 KHz,16.63 KHz,16.64 KHz,16.65 KHz,16.66 KHz,16.67 KHz,16.68 KHz,16.69 KHz,16.70 KHz,16.71 KHz,16.72 KHz,16.73 KHz,16.74 KHz,16.75 KHz,16.76 KHz,16.77 KHz,16.78 KHz,16.79 KHz,16.80 KHz,16.81 KHz,16.82 KHz,16.83 KHz,16.84 KHz,16.85 KHz,16.86 KHz,16.87 KHz,16.88 KHz,16.89 KHz,16.90 KHz,16.91 KHz,16.92 KHz,16.93 KHz,16.94 KHz,16.95 KHz,16.96 KHz,16.97 KHz,16.98 KHz,16.99 KHz,17.00 KHz,17.01 KHz,17.02 KHz,17.03 KHz,17.04 KHz,17.05 KHz,17.06 KHz,17.07 KHz,17.08 KHz,17.09 KHz,17.10 KHz,17.11 KHz,17.12 KHz,17.13 KHz,17.14 KHz,17.15 KHz,17.16 KHz,17.17 KHz,17.18 KHz,17.19 KHz,17.20 KHz,17.21 KHz,17.22 KHz,17.23 KHz,17.24 KHz,17.25 KHz,17.26 KHz,17.27 KHz,17.28 KHz,17.29 KHz,17.30 KHz,17.31 KHz,17.32 KHz,17.33 KHz,17.34 KHz,17.35 KHz,17.36 KHz,17.37 KHz,17.38 KHz,17.39 KHz,17.40 KHz,17.41 KHz,17.42 KHz,17.43 KHz,17.44 KHz,17.45 KHz,17.46 KHz,17.47 KHz,17.48 KHz,17.49 KHz,17.50 KHz,17.51 KHz,17.52 KHz,17.53 KHz,17.54 KHz,17.55 KHz,17.56 KHz,17.57 KHz,17.58 KHz,17.59 KHz,17.60 KHz,17.61 KHz,17.62 KHz,17.63 KHz,17.64 KHz,17.65 KHz,17.66 KHz,17.67 KHz,17.68 KHz,17.69 KHz,17.70 KHz,17.71 KHz,17.72 KHz,17.73 KHz,17.74 KHz,17.75 KHz,17.76 KHz,17.77 KHz,17.78 KHz,17.79 KHz,17.80 KHz,17.81 KHz,17.82 KHz,17.83 KHz,17.84 KHz,17.85 KHz,17.86 KHz,17.87 KHz,17.88 KHz,17.89 KHz,17.90 KHz,17.91 KHz,17.92 KHz,17.93 KHz,17.94 KHz,17.95 KHz,17.96 KHz,17.97 KHz,17.98 KHz,17.99 KHz,18.00 KHz,18.01 KHz,18.02 KHz,18.03 KHz,18.04 KHz,18.05 KHz,18.06 KHz,18.07 KHz,18.08 KHz,18.09 KHz,18.10 KHz,18.11 KHz,18.12 KHz,18.13 KHz,18.14 KHz,18.15 KHz,18.16 KHz,18.17 KHz,18.18 KHz,18.19 KHz,18.20 KHz,18.21 KHz,18.22 KHz,18.23 KHz,18.24 KHz,18.25 KHz,18.26 KHz,18.27 KHz,18.28 KHz,18.29 KHz,18.30 KHz,18.31 KHz,18.32 KHz,18.33 KHz,18.34 KHz,18.35 KHz,18.36 KHz,18.37 KHz,18.38 KHz,18.39 KHz,18.40 KHz,18.41 KHz,18.42 KHz,18.43 KHz,18.44 KHz,18.45 KHz,18.46 KHz,18.47 KHz,18.48 KHz,18.49 KHz,18.50 KHz,18.51 KHz,18.52 KHz,18.53 KHz,18.54 KHz,18.55 KHz,18.56 KHz,18.57 KHz,18.58 KHz,18.59 KHz,18.60 KHz,18.61 KHz,18.62 KHz,18.63 KHz,18.64 KHz,18.65 KHz,18.66 KHz,18.67 KHz,18.68 KHz,18.69 KHz,18.70 KHz,18.71 KHz,18.72 KHz,18.73 KHz,18.74 KHz,18.75 KHz,18.76 KHz,18.77 KHz,18.78 KHz,18.79 KHz,18.80 KHz,18.81 KHz,18.82 KHz,18.83 KHz,18.84 KHz,18.85 KHz,18.86 KHz,18.87 KHz,18.88 KHz,18.89 KHz,18.90 KHz,18.91 KHz,18.92 KHz,18.93 KHz,18.94 KHz,18.95 KHz,18.96 KHz,18.97 KHz,18.98 KHz,18.99 KHz,19.00 KHz,19.01 KHz,19.02 KHz,19.03 KHz,19.04 KHz,19.05 KHz,19.06 KHz,19.07 KHz,19.08 KHz,19.09 KHz,19.10 KHz,19.11 KHz,19.12 KHz,19.13 KHz,19.14 KHz,19.15 KHz,19.16 KHz,19.17 KHz,19.18 KHz,19.19 KHz,19.20 KHz,19.21 KHz,19.22 KHz,19.23 KHz,19.24 KHz,19.25 KHz,19.26 KHz,19.27 KHz,19.28 KHz,19.29 KHz,19.30 KHz,19.31 KHz,19.32 KHz,19.33 KHz,19.34 KHz,19.35 KHz,19.36 KHz,19.37 KHz,19.38 KHz,19.39 KHz,19.40 KHz,19.41 KHz,19.42 KHz,19.43 KHz,19.44 KHz,19.45 KHz,19.46 KHz,19.47 KHz,19.48 KHz,19.49 KHz,19.50 KHz,19.51 KHz,19.52 KHz,19.53 KHz,19.54 KHz,19.55 KHz,19.56 KHz,19.57 KHz,19.58 KHz,19.59 KHz,19.60 KHz,19.61 KHz,19.62 KHz,19.63 KHz,19.64 KHz,19.65 KHz,19.66 KHz,19.67 KHz,19.68 KHz,19.69 KHz,19.70 KHz,19.71 KHz,19.72 KHz,19.73 KHz,19.74 KHz,19.75 KHz,19.76 KHz,19.77 KHz,19.78 KHz,19.79 KHz,19.80 KHz,19.81 KHz,19.82 KHz,19.83 KHz,19.84 KHz,19.85 KHz,19.86 KHz,19.87 KHz,19.88 KHz,19.89 KHz,19.90 KHz,19.91 KHz,19.92 KHz,19.93 KHz,19.94 KHz,19.95 KHz,19.96 KHz,19.97 KHz,19.98 KHz,19.99 KHz,20.00 KHz,20.01 KHz,20.02 KHz,20.03 KHz,20.04 KHz,20.05 KHz,20.06 KHz,20.07 KHz,20.08 KHz,20.09 KHz,20.10 KHz,20.11 KHz,20.12 KHz,20.13 KHz,20.14 KHz,20.15 KHz,20.16 KHz,20.17 KHz,20.18 KHz,20.19 KHz,20.20 KHz,20.21 KHz,20.22 KHz,20.23 KHz,20.24 KHz,20.25 KHz,20.26 KHz,20.27 KHz,20.28 KHz,20.29 KHz,20.30 KHz,20.31 KHz,20.32 KHz,20.33 KHz,20.34 KHz,20.35 KHz,20.36 KHz,20.37 KHz,20.38 KHz,20.39 KHz,20.40 KHz,20.41 KHz,20.42 KHz,20.43 KHz,20.44 KHz,20.45 KHz,20.46 KHz,20.47 KHz,20.48 KHz,20.49 KHz,20.50 KHz,20.51 KHz,20.52 KHz,20.53 KHz,20.54 KHz,20.55 KHz,20.56 KHz,20.57 KHz,20.58 KHz,20.59 KHz,20.60 KHz,20.61 KHz,20.62 KHz,20.63 KHz,20.64 KHz,20.65 KHz,20.66 KHz,20.67 KHz,20.68 KHz,20.69 KHz,20.70 KHz,20.71 KHz,20.72 KHz,20.73 KHz,20.74 KHz,20.75 KHz,20.76 KHz,20.77 KHz,20.78 KHz,20.79 KHz,20.80 KHz,20.81 KHz,20.82 KHz,20.83 KHz,20.84 KHz,20.85 KHz,20.86 KHz,20.87 KHz,20.88 KHz,20.89 KHz,20.90 KHz,20.91 KHz,20.92 KHz,20.93 KHz,20.94 KHz,20.95 KHz,20.96 KHz,20.97 KHz,20.98 KHz,20.99 KHz,21.00 KHz,21.01 KHz,21.02 KHz,21.03 KHz,21.04 KHz,21.05 KHz,21.06 KHz,21.07 KHz,21.08 KHz,21.09 KHz,21.10 KHz,21.11 KHz,21.12 KHz,21.13 KHz,21.14 KHz,21.15 KHz,21.16 KHz,21.17 KHz,21.18 KHz,21.19 KHz,21.20 KHz,21.21 KHz,21.22 KHz,21.23 KHz,21.24 KHz,21.25 KHz,21.26 KHz,21.27 KHz,21.28 KHz,21.29 KHz,21.30 KHz,21.31 KHz,21.32 KHz,21.33 KHz,21.34 KHz,21.35 KHz,21.36 KHz,21.37 KHz,21.38 KHz,21.39 KHz,21.40 KHz,21.41 KHz,21.42 KHz,21.43 KHz,21.44 KHz,21.45 KHz,21.46 KHz,21.47 KHz,21.48 KHz,21.49 KHz,21.50 KHz,21.51 KHz,21.52 KHz,21.53 KHz,21.54 KHz,21.55 KHz,21.56 KHz,21.57 KHz,21.58 KHz,21.59 KHz,21.60 KHz,21.61 KHz,21.62 KHz,21.63 KHz,21.64 KHz,21.65 KHz,21.66 KHz,21.67 KHz,21.68 KHz,21.69 KHz,21.70 KHz,21.71 KHz,21.72 KHz,21.73 KHz,21.74 KHz,21.75 KHz,21.76 KHz,21.77 KHz,21.78 KHz,21.79 KHz,21.80 KHz,21.81 KHz,21.82 KHz,21.83 KHz,21.84 KHz,21.85 KHz,21.86 KHz,21.87 KHz,21.88 KHz,21.89 KHz,21.90 KHz,21.91 KHz,21.92 KHz,21.93 KHz,21.94 KHz,21.95 KHz,21.96 KHz,21.97 KHz,21.98 KHz,21.99 KHz,22.00 KHz,22.01 KHz,22.02 KHz,22.03 KHz,22.04 KHz,22.05 KHz,22.06 KHz,22.07 KHz,22.08 KHz,22.09 KHz,22.10 KHz,22.11 KHz,22.12 KHz,22.13 KHz,22.14 KHz,22.15 KHz,22.16 KHz,22.17 KHz,22.18 KHz,22.19 KHz,22.20 KHz,22.21 KHz,22.22 KHz,22.23 KHz,22.24 KHz,22.25 KHz,22.26 KHz,22.27 KHz,22.28 KHz,22.29 KHz,22.30 KHz,22.31 KHz,22.32 KHz,22.33 KHz,22.34 KHz,22.35 KHz,22.36 KHz,22.37 KHz,22.38 KHz,22.39 KHz,22.40 KHz,22.41 KHz,22.42 KHz,22.43 KHz,22.44 KHz,22.45 KHz,22.46 KHz,22.47 KHz,22.48 KHz,22.49 KHz,22.50 KHz,22.51 KHz,22.52 KHz,22.53 KHz,22.54 KHz,22.55 KHz,22.56 KHz,22.57 KHz,22.58 KHz,22.59 KHz,22.60 KHz,22.61 KHz,22.62 KHz,22.63 KHz,22.64 KHz,22.65 KHz,22.66 KHz,22.67 KHz,22.68 KHz,22.69 KHz,22.70 KHz,22.71 KHz,22.72 KHz,22.73 KHz,22.74 KHz,22.75 KHz,22.76 KHz,22.77 KHz,22.78 KHz,22.79 KHz,22.80 KHz,22.81 KHz,22.82 KHz,22.83 KHz,22.84 KHz,22.85 KHz,22.86 KHz,22.87 KHz,22.88 KHz,22.89 KHz,22.90 KHz,22.91 KHz,22.92 KHz,22.93 KHz,22.94 KHz,22.95 KHz,22.96 KHz,22.97 KHz,22.98 KHz,22.99 KHz,23.00 KHz,23.01 KHz,23.02 KHz,23.03 KHz,23.04 KHz,23.05 KHz,23.06 KHz,23.07 KHz,23.08 KHz,23.09 KHz,23.10 KHz,23.11 KHz,23.12 KHz,23.13 KHz,23.14 KHz,23.15 KHz,23.16 KHz,23.17 KHz,23.18 KHz,23.19 KHz,23.20 KHz,23.21 KHz,23.22 KHz,23.23 KHz,23.24 KHz,23.25 KHz,23.26 KHz,23.27 KHz,23.28 KHz,23.29 KHz,23.30 KHz,23.31 KHz,23.32 KHz,23.33 KHz,23.34 KHz,23.35 KHz,23.36 KHz,23.37 KHz,23.38 KHz,23.39 KHz,23.40 KHz,23.41 KHz,23.42 KHz,23.43 KHz,23.44 KHz,23.45 KHz,23.46 KHz,23.47 KHz,23.48 KHz,23.49 KHz,23.50 KHz,23.51 KHz,23.52 KHz,23.53 KHz,23.54 KHz,23.55 KHz,23.56 KHz,23.57 KHz,23.58 KHz,23.59 KHz,23.60 KHz,23.61 KHz,23.62 KHz,23.63 KHz,23.64 KHz,23.65 KHz,23.66 KHz,23.67 KHz,23.68 KHz,23.69 KHz,23.70 KHz,23.71 KHz,23.72 KHz,23.73 KHz,23.74 KHz,23.75 KHz,23.76 KHz,23.77 KHz,23.78 KHz,23.79 KHz,23.80 KHz,23.81 KHz,23.82 KHz,23.83 KHz,23.84 KHz,23.85 KHz,23.86 KHz,23.87 KHz,23.88 KHz,23.89 KHz,23.90 KHz,23.91 KHz,23.92 KHz,23.93 KHz,23.94 KHz,23.95 KHz,23.96 KHz,23.97 KHz,23.98 KHz,23.99 KHz,24.00 KHz,24.01 KHz,24.02 KHz,24.03 KHz,24.04 KHz,24.05 KHz,24.06 KHz,24.07 KHz,24.08 KHz,24.09 KHz,24.10 KHz,24.11 KHz,24.12 KHz,24.13 KHz,24.14 KHz,24.15 KHz,24.16 KHz,24.17 KHz,24.18 KHz,24.19 KHz,24.20 KHz,24.21 KHz,24.22 KHz,24.23 KHz,24.24 KHz,24.25 KHz,24.26 KHz,24.27 KHz,24.28 KHz,24.29 KHz,24.30 KHz,24.31 KHz,24.32 KHz,24.33 KHz,24.34 KHz,24.35 KHz,24.36 KHz,24.37 KHz,24.38 KHz,24.39 KHz,24.40 KHz,24.41 KHz,24.42 KHz,24.43 KHz,24.44 KHz,24.45 KHz,24.46 KHz,24.47 KHz,24.48 KHz,24.49 KHz,24.50 KHz,24.51 KHz,24.52 KHz,24.53 KHz,24.54 KHz,24.55 KHz,24.56 KHz,24.57 KHz,24.58 KHz,24.59 KHz,24.60 KHz,24.61 KHz,24.62 KHz,24.63 KHz,24.64 KHz,24.65 KHz,24.66 KHz,24.67 KHz,24.68 KHz,24.69 KHz,24.70 KHz,24.71 KHz,24.72 KHz,24.73 KHz,24.74 KHz,24.75 KHz,24.76 KHz,24.77 KHz,24.78 KHz,24.79 KHz,24.80 KHz,24.81 KHz,24.82 KHz,24.83 KHz,24.84 KHz,24.85 KHz,24.86 KHz,24.87 KHz,24.88 KHz,24.89 KHz,24.90 KHz,24.91 KHz,24.92 KHz,24.93 KHz,24.94 KHz,24.95 KHz,24.96 KHz,24.97 KHz,24.98 KHz,24.99 KHz,25.00 KHz,25.01 KHz,25.02 KHz,25.03 KHz,25.04 KHz,25.05 KHz,25.06 KHz,25.07 KHz,25.08 KHz,25.09 KHz,25.10 KHz,25.11 KHz,25.12 KHz,25.13 KHz,25.14 KHz,25.15 KHz,25.16 KHz,25.17 KHz,25.18 KHz,25.19 KHz,25.20 KHz,25.21 KHz,25.22 KHz,25.23 KHz,25.24 KHz,25.25 KHz,25.26 KHz,25.27 KHz,25.28 KHz,25.29 KHz,25.30 KHz,25.31 KHz,25.32 KHz,25.33 KHz,25.34 KHz,25.35 KHz,25.36 KHz,25.37 KHz,25.38 KHz,25.39 KHz,25.40 KHz,25.41 KHz,25.42 KHz,25.43 KHz,25.44 KHz,25.45 KHz,25.46 KHz,25.47 KHz,25.48 KHz,25.49 KHz,25.50 KHz,25.51 KHz,25.52 KHz,25.53 KHz,25.54 KHz,25.55 KHz,25.56 KHz,25.57 KHz,25.58 KHz,25.59 KHz,25.60 KHz,25.61 KHz,25.62 KHz,25.63 KHz,25.64 KHz,25.65 KHz,25.66 KHz,25.67 KHz,25.68 KHz,25.69 KHz,25.70 KHz,25.71 KHz,25.72 KHz,25.73 KHz,25.74 KHz,25.75 KHz,25.76 KHz,25.77 KHz,25.78 KHz,25.79 KHz,25.80 KHz,25.81 KHz,25.82 KHz,25.83 KHz,25.84 KHz,25.85 KHz,25.86 KHz,25.87 KHz,25.88 KHz,25.89 KHz,25.90 KHz,25.91 KHz,25.92 KHz,25.93 KHz,25.94 KHz,25.95 KHz,25.96 KHz,25.97 KHz,25.98 KHz,25.99 KHz,26.00 KHz,26.01 KHz,26.02 KHz,26.03 KHz,26.04 KHz,26.05 KHz,26.06 KHz,26.07 KHz,26.08 KHz,26.09 KHz,26.10 KHz,26.11 KHz,26.12 KHz,26.13 KHz,26.14 KHz,26.15 KHz,26.16 KHz,26.17 KHz,26.18 KHz,26.19 KHz,26.20 KHz,26.21 KHz,26.22 KHz,26.23 KHz,26.24 KHz,26.25 KHz,26.26 KHz,26.27 KHz,26.28 KHz,26.29 KHz,26.30 KHz,26.31 KHz,26.32 KHz,26.33 KHz,26.34 KHz,26.35 KHz,26.36 KHz,26.37 KHz,26.38 KHz,26.39 KHz,26.40 KHz,26.41 KHz,26.42 KHz,26.43 KHz,26.44 KHz,26.45 KHz,26.46 KHz,26.47 KHz,26.48 KHz,26.49 KHz,26.50 KHz,26.51 KHz,26.52 KHz,26.53 KHz,26.54 KHz,26.55 KHz,26.56 KHz,26.57 KHz,26.58 KHz,26.59 KHz,26.60 KHz,26.61 KHz,26.62 KHz,26.63 KHz,26.64 KHz,26.65 KHz,26.66 KHz,26.67 KHz,26.68 KHz,26.69 KHz,26.70 KHz,26.71 KHz,26.72 KHz,26.73 KHz,26.74 KHz,26.75 KHz,26.76 KHz,26.77 KHz,26.78 KHz,26.79 KHz,26.80 KHz,26.81 KHz,26.82 KHz,26.83 KHz,26.84 KHz,26.85 KHz,26.86 KHz,26.87 KHz,26.88 KHz,26.89 KHz,26.90 KHz,26.91 KHz,26.92 KHz,26.93 KHz,26.94 KHz,26.95 KHz,26.96 KHz,26.97 KHz,26.98 KHz,26.99 KHz,27.00 KHz,27.01 KHz,27.02 KHz,27.03 KHz,27.04 KHz,27.05 KHz,27.06 KHz,27.07 KHz,27.08 KHz,27.09 KHz,27.10 KHz,27.11 KHz,27.12 KHz,27.13 KHz,27.14 KHz,27.15 KHz,27.16 KHz,27.17 KHz,27.18 KHz,27.19 KHz,27.20 KHz,27.21 KHz,27.22 KHz,27.23 KHz,27.24 KHz,27.25 KHz,27.26 KHz,27.27 KHz,27.28 KHz,27.29 KHz,27.30 KHz,27.31 KHz,27.32 KHz,27.33 KHz,27.34 KHz,27.35 KHz,27.36 KHz,27.37 KHz,27.38 KHz,27.39 KHz,27.40 KHz,27.41 KHz,27.42 KHz,27.43 KHz,27.44 KHz,27.45 KHz,27.46 KHz,27.47 KHz,27.48 KHz,27.49 KHz,27.50 KHz,27.51 KHz,27.52 KHz,27.53 KHz,27.54 KHz,27.55 KHz,27.56 KHz,27.57 KHz,27.58 KHz,27.59 KHz,27.60 KHz,27.61 KHz,27.62 KHz,27.63 KHz,27.64 KHz,27.65 KHz,27.66 KHz,27.67 KHz,27.68 KHz,27.69 KHz,27.70 KHz,27.71 KHz,27.72 KHz,27.73 KHz,27.74 KHz,27.75 KHz,27.76 KHz,27.77 KHz,27.78 KHz,27.79 KHz,27.80 KHz,27.81 KHz,27.82 KHz,27.83 KHz,27.84 KHz,27.85 KHz,27.86 KHz,27.87 KHz,27.88 KHz,27.89 KHz,27.90 KHz,27.91 KHz,27.92 KHz,27.93 KHz,27.94 KHz,27.95 KHz,27.96 KHz,27.97 KHz,27.98 KHz,27.99 KHz,28.00 KHz,28.01 KHz,28.02 KHz,28.03 KHz,28.04 KHz,28.05 KHz,28.06 KHz,28.07 KHz,28.08 KHz,28.09 KHz,28.10 KHz,28.11 KHz,28.12 KHz,28.13 KHz,28.14 KHz,28.15 KHz,28.16 KHz,28.17 KHz,28.18 KHz,28.19 KHz,28.20 KHz,28.21 KHz,28.22 KHz,28.23 KHz,28.24 KHz,28.25 KHz,28.26 KHz,28.27 KHz,28.28 KHz,28.29 KHz,28.30 KHz,28.31 KHz,28.32 KHz,28.33 KHz,28.34 KHz,28.35 KHz,28.36 KHz,28.37 KHz,28.38 KHz,28.39 KHz,28.40 KHz,28.41 KHz,28.42 KHz,28.43 KHz,28.44 KHz,28.45 KHz,28.46 KHz,28.47 KHz,28.48 KHz,28.49 KHz,28.50 KHz,28.51 KHz,28.52 KHz,28.53 KHz,28.54 KHz,28.55 KHz,28.56 KHz,28.57 KHz,28.58 KHz,28.59 KHz,28.60 KHz,28.61 KHz,28.62 KHz,28.63 KHz,28.64 KHz,28.65 KHz,28.66 KHz,28.67 KHz,28.68 KHz,28.69 KHz,28.70 KHz,28.71 KHz,28.72 KHz,28.73 KHz,28.74 KHz,28.75 KHz,28.76 KHz,28.77 KHz,28.78 KHz,28.79 KHz,28.80 KHz,28.81 KHz,28.82 KHz,28.83 KHz,28.84 KHz,28.85 KHz,28.86 KHz,28.87 KHz,28.88 KHz,28.89 KHz,28.90 KHz,28.91 KHz,28.92 KHz,28.93 KHz,28.94 KHz,28.95 KHz,28.96 KHz,28.97 KHz,28.98 KHz,28.99 KHz,29.00 KHz,29.01 KHz,29.02 KHz,29.03 KHz,29.04 KHz,29.05 KHz,29.06 KHz,29.07 KHz,29.08 KHz,29.09 KHz,29.10 KHz,29.11 KHz,29.12 KHz,29.13 KHz,29.14 KHz,29.15 KHz,29.16 KHz,29.17 KHz,29.18 KHz,29.19 KHz,29.20 KHz,29.21 KHz,29.22 KHz,29.23 KHz,29.24 KHz,29.25 KHz,29.26 KHz,29.27 KHz,29.28 KHz,29.29 KHz,29.30 KHz,29.31 KHz,29.32 KHz,29.33 KHz,29.34 KHz,29.35 KHz,29.36 KHz,29.37 KHz,29.38 KHz,29.39 KHz,29.40 KHz,29.41 KHz,29.42 KHz,29.43 KHz,29.44 KHz,29.45 KHz,29.46 KHz,29.47 KHz,29.48 KHz,29.49 KHz,29.50 KHz,29.51 KHz,29.52 KHz,29.53 KHz,29.54 KHz,29.55 KHz,29.56 KHz,29.57 KHz,29.58 KHz,29.59 KHz,29.60 KHz,29.61 KHz,29.62 KHz,29.63 KHz,29.64 KHz,29.65 KHz,29.66 KHz,29.67 KHz,29.68 KHz,29.69 KHz,29.70 KHz,29.71 KHz,29.72 KHz,29.73 KHz,29.74 KHz,29.75 KHz,29.76 KHz,29.77 KHz,29.78 KHz,29.79 KHz,29.80 KHz,29.81 KHz,29.82 KHz,29.83 KHz,29.84 KHz,29.85 KHz,29.86 KHz,29.87 KHz,29.88 KHz,29.89 KHz,29.90 KHz,29.91 KHz,29.92 KHz,29.93 KHz,29.94 KHz,29.95 KHz,29.96 KHz,29.97 KHz,29.98 KHz,29.99 KHz,30.00 KHz,30.01 KHz,30.02 KHz,30.03 KHz,30.04 KHz,30.05 KHz,30.06 KHz,30.07 KHz,30.08 KHz,30.09 KHz,30.10 KHz,30.11 KHz,30.12 KHz,30.13 KHz,30.14 KHz,30.15 KHz,30.16 KHz,30.17 KHz,30.18 KHz,30.19 KHz,30.20 KHz,30.21 KHz,30.22 KHz,30.23 KHz,30.24 KHz,30.25 KHz,30.26 KHz,30.27 KHz,30.28 KHz,30.29 KHz,30.30 KHz,30.31 KHz,30.32 KHz,30.33 KHz,30.34 KHz,30.35 KHz,30.36 KHz,30.37 KHz,30.38 KHz,30.39 KHz,30.40 KHz,30.41 KHz,30.42 KHz,30.43 KHz,30.44 KHz,30.45 KHz,30.46 KHz,30.47 KHz,30.48 KHz,30.49 KHz,30.50 KHz,30.51 KHz,30.52 KHz,30.53 KHz,30.54 KHz,30.55 KHz,30.56 KHz,30.57 KHz,30.58 KHz,30.59 KHz,30.60 KHz,30.61 KHz,30.62 KHz,30.63 KHz,30.64 KHz,30.65 KHz,30.66 KHz,30.67 KHz,30.68 KHz,30.69 KHz,30.70 KHz,30.71 KHz,30.72 KHz,30.73 KHz,30.74 KHz,30.75 KHz,30.76 KHz,30.77 KHz,30.78 KHz,30.79 KHz,30.80 KHz,30.81 KHz,30.82 KHz,30.83 KHz,30.84 KHz,30.85 KHz,30.86 KHz,30.87 KHz,30.88 KHz,30.89 KHz,30.90 KHz,30.91 KHz,30.92 KHz,30.93 KHz,30.94 KHz,30.95 KHz,30.96 KHz,30.97 KHz,30.98 KHz,30.99 KHz,31.00 KHz,31.01 KHz,31.02 KHz,31.03 KHz,31.04 KHz,31.05 KHz,31.06 KHz,31.07 KHz,31.08 KHz,31.09 KHz,31.10 KHz,31.11 KHz,31.12 KHz,31.13 KHz,31.14 KHz,31.15 KHz,31.16 KHz,31.17 KHz,31.18 KHz,31.19 KHz,31.20 KHz,31.21 KHz,31.22 KHz,31.23 KHz,31.24 KHz,31.25 KHz,31.26 KHz,31.27 KHz,31.28 KHz,31.29 KHz,31.30 KHz,31.31 KHz,31.32 KHz,31.33 KHz,31.34 KHz,31.35 KHz,31.36 KHz,31.37 KHz,31.38 KHz,31.39 KHz,31.40 KHz,31.41 KHz,31.42 KHz,31.43 KHz,31.44 KHz,31.45 KHz,31.46 KHz,31.47 KHz,31.48 KHz,31.49 KHz,31.50 KHz,31.51 KHz,31.52 KHz,31.53 KHz,31.54 KHz,31.55 KHz,31.56 KHz,31.57 KHz,31.58 KHz,31.59 KHz,31.60 KHz,31.61 KHz,31.62 KHz,31.63 KHz,31.64 KHz,31.65 KHz,31.66 KHz,31.67 KHz,31.68 KHz,31.69 KHz,31.70 KHz,31.71 KHz,31.72 KHz,31.73 KHz,31.74 KHz,31.75 KHz,31.76 KHz,31.77 KHz,31.78 KHz,31.79 KHz,31.80 KHz,31.81 KHz,31.82 KHz,31.83 KHz,31.84 KHz,31.85 KHz,31.86 KHz,31.87 KHz,31.88 KHz,31.89 KHz,31.90 KHz,31.91 KHz,31.92 KHz,31.93 KHz,31.94 KHz,31.95 KHz,31.96 KHz,31.97 KHz,31.98 KHz,31.99 KHz,32.00 KHz,32.01 KHz,32.02 KHz,32.03 KHz,32.04 KHz,32.05 KHz,32.06 KHz,32.07 KHz,32.08 KHz,32.09 KHz,32.10 KHz,32.11 KHz,32.12 KHz,32.13 KHz,32.14 KHz,32.15 KHz,32.16 KHz,32.17 KHz,32.18 KHz,32.19 KHz,32.20 KHz,32.21 KHz,32.22 KHz,32.23 KHz,32.24 KHz,32.25 KHz,32.26 KHz,32.27 KHz,32.28 KHz,32.29 KHz,32.30 KHz,32.31 KHz,32.32 KHz,32.33 KHz,32.34 KHz,32.35 KHz,32.36 KHz,32.37 KHz,32.38 KHz,32.39 KHz,32.40 KHz,32.41 KHz,32.42 KHz,32.43 KHz,32.44 KHz,32.45 KHz,32.46 KHz,32.47 KHz,32.48 KHz,32.49 KHz,32.50 KHz,32.51 KHz,32.52 KHz,32.53 KHz,32.54 KHz,32.55 KHz,32.56 KHz,32.57 KHz,32.58 KHz,32.59 KHz,32.60 KHz,32.61 KHz,32.62 KHz,32.63 KHz,32.64 KHz,32.65 KHz,32.66 KHz,32.67 KHz,32.68 KHz,32.69 KHz,32.70 KHz,32.71 KHz,32.72 KHz,32.73 KHz,32.74 KHz,32.75 KHz,32.76 KHz,32.77 KHz,32.78 KHz,32.79 KHz,32.80 KHz,32.81 KHz,32.82 KHz,32.83 KHz,32.84 KHz,32.85 KHz,32.86 KHz,32.87 KHz,32.88 KHz,32.89 KHz,32.90 KHz,32.91 KHz,32.92 KHz,32.93 KHz,32.94 KHz,32.95 KHz,32.96 KHz,32.97 KHz,32.98 KHz,32.99 KHz,33.00 KHz,33.01 KHz,33.02 KHz,33.03 KHz,33.04 KHz,33.05 KHz,33.06 KHz,33.07 KHz,33.08 KHz,33.09 KHz,33.10 KHz,33.11 KHz,33.12 KHz,33.13 KHz,33.14 KHz,33.15 KHz,33.16 KHz,33.17 KHz,33.18 KHz,33.19 KHz,33.20 KHz,33.21 KHz,33.22 KHz,33.23 KHz,33.24 KHz,33.25 KHz,33.26 KHz,33.27 KHz,33.28 KHz,33.29 KHz,33.30 KHz,33.31 KHz,33.32 KHz,33.33 KHz,33.34 KHz,33.35 KHz,33.36 KHz,33.37 KHz,33.38 KHz,33.39 KHz,33.40 KHz,33.41 KHz,33.42 KHz,33.43 KHz,33.44 KHz,33.45 KHz,33.46 KHz,33.47 KHz,33.48 KHz,33.49 KHz,33.50 KHz,33.51 KHz,33.52 KHz,33.53 KHz,33.54 KHz,33.55 KHz,33.56 KHz,33.57 KHz,33.58 KHz,33.59 KHz,33.60 KHz,33.61 KHz,33.62 KHz,33.63 KHz,33.64 KHz,33.65 KHz,33.66 KHz,33.67 KHz,33.68 KHz,33.69 KHz,33.70 KHz,33.71 KHz,33</t>
         </is>
       </c>
       <c r="C5" s="61" t="n"/>
@@ -2068,35 +2068,15 @@
       </c>
     </row>
     <row r="11" ht="13.55" customHeight="1" s="50">
-      <c r="A11" s="41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B11" s="41" t="inlineStr">
-        <is>
-          <t>Cascade connection</t>
-        </is>
-      </c>
-      <c r="C11" s="41" t="inlineStr">
-        <is>
-          <t>Series impedance</t>
-        </is>
-      </c>
-      <c r="D11" s="41" t="inlineStr">
-        <is>
-          <t>Resistor</t>
-        </is>
-      </c>
-      <c r="E11" s="41" t="inlineStr">
-        <is>
-          <t>100K</t>
-        </is>
-      </c>
-      <c r="F11" s="41" t="inlineStr"/>
-      <c r="G11" s="41" t="inlineStr"/>
-      <c r="H11" s="41" t="inlineStr"/>
-      <c r="I11" s="41" t="inlineStr"/>
+      <c r="A11" s="41" t="n"/>
+      <c r="B11" s="41" t="n"/>
+      <c r="C11" s="41" t="n"/>
+      <c r="D11" s="41" t="n"/>
+      <c r="E11" s="41" t="n"/>
+      <c r="F11" s="41" t="n"/>
+      <c r="G11" s="41" t="n"/>
+      <c r="H11" s="41" t="n"/>
+      <c r="I11" s="41" t="n"/>
       <c r="J11" s="41" t="n"/>
       <c r="K11" s="41" t="n"/>
       <c r="L11" s="41" t="n"/>

</xml_diff>